<commit_message>
bach update express charge list + export
</commit_message>
<xml_diff>
--- a/resources/excels/ShiftExport.xlsx
+++ b/resources/excels/ShiftExport.xlsx
@@ -92,12 +92,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="MS PGothic"/>
+      <name val="ＭＳ ゴシック"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="ＭＳ ゴシック"/>
+      <name val="MS PGothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -198,22 +199,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +433,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -485,115 +486,115 @@
       <c r="A5" s="2">
         <v>144</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:10" ht="14.25" customHeight="1"/>
@@ -1589,6 +1590,6 @@
     <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bach repository cash_in, cash_in_statical, cash_in_history
</commit_message>
<xml_diff>
--- a/resources/excels/ShiftExport.xlsx
+++ b/resources/excels/ShiftExport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>シフト表</t>
   </si>
@@ -46,18 +46,12 @@
   <si>
     <t>仏滅</t>
   </si>
-  <si>
-    <t>管理職・リーダー</t>
-  </si>
-  <si>
-    <t>Name1</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -89,19 +83,8 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="ＭＳ ゴシック"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="MS PGothic"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,18 +99,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFDDC8"/>
-        <bgColor rgb="FFFFDDC8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -180,41 +157,26 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +395,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -444,26 +406,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
@@ -483,118 +445,109 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="2">
-        <v>144</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:10" ht="14.25" customHeight="1"/>

</xml_diff>